<commit_message>
Changed name and structure of input data
</commit_message>
<xml_diff>
--- a/Video_links.xlsx
+++ b/Video_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roelofblommaert/Thesis-2024/Thesis-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E124DE98-376D-8F4D-83DF-724CC1E87035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E03CB90-9E92-6840-A7A6-9FCCF8591EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{9837DC1C-77C1-9247-8046-66082B9B7CFD}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17300" xr2:uid="{9837DC1C-77C1-9247-8046-66082B9B7CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Doordash</t>
   </si>
   <si>
-    <t>Video_id</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=vQ88JB-lgtQ&amp;t=5s&amp;ab_channel=DisneyPlus</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=Ej7fYDHlCbA&amp;ab_channel=CoorsLight</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EDA2698-6B55-6F46-8306-C54161FB3AF5}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,7 +801,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -810,10 +810,10 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -821,13 +821,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <v>2024</v>
@@ -838,13 +838,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>2024</v>
@@ -855,13 +855,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
       <c r="F4">
         <v>2024</v>
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>2024</v>
@@ -889,13 +889,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
       </c>
       <c r="F6">
         <v>2024</v>
@@ -906,13 +906,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
       </c>
       <c r="F7">
         <v>2024</v>
@@ -923,13 +923,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>2024</v>
@@ -940,13 +940,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9">
         <v>2024</v>
@@ -957,13 +957,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10">
         <v>2024</v>
@@ -974,13 +974,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11">
         <v>2024</v>
@@ -991,13 +991,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12">
         <v>2024</v>
@@ -1008,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F13">
         <v>2024</v>
@@ -1025,13 +1025,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>2024</v>
@@ -1042,13 +1042,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
         <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
       </c>
       <c r="F15">
         <v>2024</v>
@@ -1059,13 +1059,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16">
         <v>2024</v>
@@ -1076,13 +1076,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
         <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
       </c>
       <c r="F17">
         <v>2024</v>
@@ -1093,13 +1093,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18">
         <v>2024</v>
@@ -1110,13 +1110,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19">
         <v>2024</v>
@@ -1127,13 +1127,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20">
         <v>2024</v>
@@ -1144,13 +1144,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
         <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>42</v>
       </c>
       <c r="F21">
         <v>2024</v>
@@ -1161,13 +1161,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22">
         <v>2024</v>
@@ -1178,13 +1178,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F23">
         <v>2024</v>
@@ -1195,13 +1195,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24">
         <v>2024</v>
@@ -1212,13 +1212,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
         <v>48</v>
-      </c>
-      <c r="D25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" t="s">
-        <v>49</v>
       </c>
       <c r="F25">
         <v>2024</v>
@@ -1229,13 +1229,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F26">
         <v>2024</v>
@@ -1246,13 +1246,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27">
         <v>2024</v>
@@ -1263,13 +1263,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
         <v>55</v>
-      </c>
-      <c r="E28" t="s">
-        <v>56</v>
       </c>
       <c r="F28">
         <v>2024</v>
@@ -1280,13 +1280,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
         <v>58</v>
-      </c>
-      <c r="D29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
       </c>
       <c r="F29">
         <v>2024</v>
@@ -1297,13 +1297,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F30">
         <v>2024</v>
@@ -1314,13 +1314,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
         <v>61</v>
-      </c>
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" t="s">
-        <v>62</v>
       </c>
       <c r="F31">
         <v>2024</v>
@@ -1331,13 +1331,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
         <v>63</v>
-      </c>
-      <c r="D32" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" t="s">
-        <v>64</v>
       </c>
       <c r="F32">
         <v>2024</v>
@@ -1354,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33">
         <v>2024</v>
@@ -1365,13 +1365,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F34">
         <v>2024</v>
@@ -1382,13 +1382,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
         <v>69</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>70</v>
-      </c>
-      <c r="E35" t="s">
-        <v>71</v>
       </c>
       <c r="F35">
         <v>2024</v>
@@ -1399,13 +1399,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
         <v>72</v>
-      </c>
-      <c r="D36" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" t="s">
-        <v>73</v>
       </c>
       <c r="F36">
         <v>2024</v>
@@ -1416,13 +1416,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F37">
         <v>2024</v>
@@ -1433,13 +1433,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" t="s">
         <v>76</v>
-      </c>
-      <c r="D38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" t="s">
-        <v>77</v>
       </c>
       <c r="F38">
         <v>2024</v>
@@ -1450,13 +1450,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F39">
         <v>2024</v>
@@ -1467,13 +1467,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F40">
         <v>2024</v>
@@ -1484,13 +1484,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" t="s">
         <v>82</v>
-      </c>
-      <c r="D41" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" t="s">
-        <v>83</v>
       </c>
       <c r="F41">
         <v>2024</v>
@@ -1501,13 +1501,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" t="s">
         <v>84</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>85</v>
-      </c>
-      <c r="E42" t="s">
-        <v>86</v>
       </c>
       <c r="F42">
         <v>2024</v>
@@ -1518,13 +1518,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F43">
         <v>2024</v>
@@ -1535,13 +1535,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" t="s">
         <v>90</v>
-      </c>
-      <c r="D44" t="s">
-        <v>90</v>
-      </c>
-      <c r="E44" t="s">
-        <v>91</v>
       </c>
       <c r="F44">
         <v>2024</v>
@@ -1552,13 +1552,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" t="s">
         <v>94</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>95</v>
-      </c>
-      <c r="E45" t="s">
-        <v>96</v>
       </c>
       <c r="F45">
         <v>2024</v>
@@ -1569,13 +1569,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F46">
         <v>2024</v>
@@ -1586,13 +1586,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" t="s">
         <v>99</v>
-      </c>
-      <c r="D47" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47" t="s">
-        <v>100</v>
       </c>
       <c r="F47">
         <v>2024</v>
@@ -1603,13 +1603,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" t="s">
         <v>101</v>
-      </c>
-      <c r="D48" t="s">
-        <v>101</v>
-      </c>
-      <c r="E48" t="s">
-        <v>102</v>
       </c>
       <c r="F48">
         <v>2024</v>
@@ -1620,13 +1620,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" t="s">
         <v>103</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>104</v>
-      </c>
-      <c r="E49" t="s">
-        <v>105</v>
       </c>
       <c r="F49">
         <v>2024</v>
@@ -1637,13 +1637,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" t="s">
         <v>107</v>
       </c>
-      <c r="D50" t="s">
-        <v>108</v>
-      </c>
       <c r="E50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F50">
         <v>2024</v>
@@ -1654,13 +1654,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F51">
         <v>2024</v>
@@ -1671,13 +1671,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" t="s">
+        <v>110</v>
+      </c>
+      <c r="E52" t="s">
         <v>111</v>
-      </c>
-      <c r="D52" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" t="s">
-        <v>112</v>
       </c>
       <c r="F52">
         <v>2024</v>
@@ -1688,13 +1688,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" t="s">
         <v>113</v>
-      </c>
-      <c r="D53" t="s">
-        <v>113</v>
-      </c>
-      <c r="E53" t="s">
-        <v>114</v>
       </c>
       <c r="F53">
         <v>2024</v>
@@ -1720,7 +1720,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1728,22 +1728,22 @@
         <v>2024</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed data from 2024-2020
</commit_message>
<xml_diff>
--- a/Video_links.xlsx
+++ b/Video_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roelofblommaert/Thesis-2024/Thesis-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8087C141-968A-3A4F-80BC-9C8D6CF90A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CCC776-AA04-9D43-9A04-A3BFE02E660A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{9837DC1C-77C1-9247-8046-66082B9B7CFD}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17380" xr2:uid="{9837DC1C-77C1-9247-8046-66082B9B7CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="417">
   <si>
     <t>Brand</t>
   </si>
@@ -868,6 +868,426 @@
   </si>
   <si>
     <t>ULTRA Club | Full Swing Gossip</t>
+  </si>
+  <si>
+    <t>Ambulance - Only In Theaters April 8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ev82iHoLk8s&amp;ab_channel=UniversalPictures</t>
+  </si>
+  <si>
+    <t>NOPE | SBLVI SPOT</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-x__vh1H0dQ&amp;ab_channel=UniversalPictures</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: The Rings of Power - Title Announcement | Prime Video</t>
+  </si>
+  <si>
+    <t>Prime Video</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QhqGCPMfkNM&amp;ab_channel=PrimeVideo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6rcw6GdCQC8&amp;ab_channel=MichelobULTRA</t>
+  </si>
+  <si>
+    <t>Michelob ULTRA | Welcome to Superior Bowl</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AV8NXzi5Lj0&amp;ab_channel=DisneyPlus</t>
+  </si>
+  <si>
+    <t>Disney+ Has All the GOATs | Disney+</t>
+  </si>
+  <si>
+    <t>‘Geen Compromissen’ Finale Spot | Polestar</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=B4QI0VzbkHk&amp;t=2s&amp;ab_channel=PolestarCars</t>
+  </si>
+  <si>
+    <t>PoleStar</t>
+  </si>
+  <si>
+    <t>Polestar Cars</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KM3Yx-5Ymiw&amp;t=2s&amp;ab_channel=MarvelEntertainment</t>
+  </si>
+  <si>
+    <t>Marvel</t>
+  </si>
+  <si>
+    <t>Marvel Entertainment</t>
+  </si>
+  <si>
+    <t>Big Game TV Spot | Marvel Studios’ Moon Knight | Disney+</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PqgaQ9WnJSI&amp;ab_channel=CueHealth</t>
+  </si>
+  <si>
+    <t>Meet Cue: A New Smart Device for Your Health</t>
+  </si>
+  <si>
+    <t>Cue Health</t>
+  </si>
+  <si>
+    <t>Flamin' Hot I Super Bowl LVI TV Spot</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UihVmkDISsg&amp;ab_channel=Cheetos</t>
+  </si>
+  <si>
+    <t>Cheetos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rjZ_O-c3QRw&amp;ab_channel=PringlesU.S.</t>
+  </si>
+  <si>
+    <t>Pringles | Stuck In :90</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nUC1QA5gRcU&amp;ab_channel=BMWUSA</t>
+  </si>
+  <si>
+    <t>Zeus &amp; Hera | BMW USA (Official Video)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X5-nAFdvg7c&amp;ab_channel=SKECHERS</t>
+  </si>
+  <si>
+    <t>Willie Nelson for Skechers – “On the Road” Big Game commercial</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Vs0YHD0JoCk&amp;ab_channel=BudLight</t>
+  </si>
+  <si>
+    <t>Bud Light Seltzer Hard Soda - Land of Loud Flavors (:60s)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YPV7X8_zKfc&amp;ab_channel=TacoBell</t>
+  </si>
+  <si>
+    <t>Taco Bell</t>
+  </si>
+  <si>
+    <t>The Grande Escape (Commercial) | Taco Bell</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0XXmCAwO3qg&amp;ab_channel=MichelobULTRA</t>
+  </si>
+  <si>
+    <t>Superior Bowl | Caddy</t>
+  </si>
+  <si>
+    <t>Stuff | Made to Travel | 30 | Expedia</t>
+  </si>
+  <si>
+    <t>Expedia</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CMaispXEh94&amp;ab_channel=Expedia</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YchR7cbFuAU&amp;ab_channel=Booking.com</t>
+  </si>
+  <si>
+    <t>Idris for Booking.com - the #1 accommodation site on Planet Earth.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=x_UgHZdjgvQ&amp;ab_channel=ToyotaGlobal</t>
+  </si>
+  <si>
+    <t>Toyota Global</t>
+  </si>
+  <si>
+    <t>Start Your Impossible | Brothers | Toyota</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fwnbHVYgprA&amp;ab_channel=WeatherTech</t>
+  </si>
+  <si>
+    <t>WeatherTech Big Game Commercial 2022 - Special Ops: Fit Crew</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YpKYj8edUOg&amp;ab_channel=Carvana</t>
+  </si>
+  <si>
+    <t>Carvana - Official Big Game Commercial 2022 - “Oversharing Mom”</t>
+  </si>
+  <si>
+    <t>Carvana</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_wkvH0qBMP8&amp;ab_channel=Reddit</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
+  <si>
+    <t>Wow, that actually worked.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vDHNMqOLw_o&amp;ab_channel=Dr.Squatch</t>
+  </si>
+  <si>
+    <t>Dr. Squatch</t>
+  </si>
+  <si>
+    <t>Dr. Squatch Super Bowl LV Commercial 2021 - You're Not A Dish</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5L6juLUkwuw&amp;ab_channel=T-Mobile</t>
+  </si>
+  <si>
+    <t>Tom Brady &amp; Rob Gronkowski | Big Game Ad | #TheGOATin5G | T-Mobile</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eB1m-WogYeg&amp;ab_channel=UniversalPictures</t>
+  </si>
+  <si>
+    <t>Old - The Big Game Spot [HD]</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9cEiYQwYLPk&amp;ab_channel=MountainDew</t>
+  </si>
+  <si>
+    <t>WIN $1MILLION! | 2021 “MTN DEW MAJOR MELON Bottle Count” w/ John Cena</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yfLz54hzpPs&amp;ab_channel=BassProShops</t>
+  </si>
+  <si>
+    <t>Bass Pro Shops and Cabela’s Super Bowl Commercial 2021: Get Back to Nature</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7ZUT9ftBWI8&amp;ab_channel=JimmyJohn%27s</t>
+  </si>
+  <si>
+    <t>Meet the King :30 | Jimmy John’s</t>
+  </si>
+  <si>
+    <t>Jimmy John's</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3F1KdZCJ6Vg&amp;ab_channel=MichelobULTRA</t>
+  </si>
+  <si>
+    <t>Michelob ULTRA Organic Seltzer | "All-Star Cast"</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_nwSmOEiDls&amp;ab_channel=Inspiration4</t>
+  </si>
+  <si>
+    <t>Inspiration4</t>
+  </si>
+  <si>
+    <t>Super Bowl Ad: Join The First All-Civilian Space Mission | Inspiration4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dgu5ppBIr9A&amp;t=1s&amp;ab_channel=SKECHERS</t>
+  </si>
+  <si>
+    <t>Tony Romo for Skechers Max Cushioning</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zN8naTqX3TI&amp;ab_channel=Dexcom</t>
+  </si>
+  <si>
+    <t>Dexcom Official Big Game Commercial 2021 with Nick Jonas</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aaC457-XO9M&amp;ab_channel=Huggies%C2%AEBrand</t>
+  </si>
+  <si>
+    <t>Welcome to the World, Baby | Huggies® Official Big Game Commercial</t>
+  </si>
+  <si>
+    <t>Huggies® Brand</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xxNxqveseyI&amp;ab_channel=amazon</t>
+  </si>
+  <si>
+    <t>Amazon’s Big Game Commercial: Alexa’s Body</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=R2Wkk-TDnRQ&amp;ab_channel=WeatherTech</t>
+  </si>
+  <si>
+    <t>WeatherTech We Never Left Super Bowl Commercial 2021</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rF6Jjm5547k&amp;ab_channel=WeatherTech</t>
+  </si>
+  <si>
+    <t>WeatherTech Family Super Bowl Commercial 2021</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eppEgrmFacQ&amp;ab_channel=MichelobULTRA</t>
+  </si>
+  <si>
+    <t>Michelob ULTRA | “Happy” Super Bowl</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=BkXHqihY4RE&amp;ab_channel=ChipotleMexicanGrill</t>
+  </si>
+  <si>
+    <t>Chipotle | Can a Burrito Change the World?</t>
+  </si>
+  <si>
+    <t>Chipotle Mexican Grill</t>
+  </si>
+  <si>
+    <t>Chipotle</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=62EB4JniuTc&amp;ab_channel=MarvelEntertainment</t>
+  </si>
+  <si>
+    <t>“Big Game” Spot | Marvel Studios | Disney+</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7BgcG_l9J0A&amp;ab_channel=JamesBond007</t>
+  </si>
+  <si>
+    <t>James Bond 007</t>
+  </si>
+  <si>
+    <t>NO TIME TO DIE | Official Game Day Spot 2020</t>
+  </si>
+  <si>
+    <t>Metro-Goldwyn-Mayer </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MoVpgtAJHfU&amp;ab_channel=Mr.Peanut</t>
+  </si>
+  <si>
+    <t>Mr. Peanut</t>
+  </si>
+  <si>
+    <t>Tribute | Planters | 2020 Big Game Commercial</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lTL3OZkVMHQ&amp;ab_channel=MarvelEntertainment</t>
+  </si>
+  <si>
+    <t>Marvel Studios' Black Widow | Big Game Spot</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pPZDV1eCI0c&amp;ab_channel=TheFastSaga</t>
+  </si>
+  <si>
+    <t>F9 - In Theaters April 2021 (Hallelujah) [HD]</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NSmkA7hcNjs&amp;t=5s&amp;ab_channel=ParamountPictures</t>
+  </si>
+  <si>
+    <t>Top Gun: Maverick (2022) – Big Game Spot – Paramount Pictures</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-gAZRN3SCBw&amp;ab_channel=Coca-Cola</t>
+  </si>
+  <si>
+    <t>Coca-Cola</t>
+  </si>
+  <si>
+    <t>Coca-Cola Energy - Show Up ft. Jonah Hill &amp; Martin Scorsese</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=mi5RoP1-8-I&amp;ab_channel=ParamountPictures</t>
+  </si>
+  <si>
+    <t>A Quiet Place Part II (2020) - Big Game Spot - Paramount Pictures</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8btMI_N8v8U&amp;ab_channel=WaltDisneyStudios</t>
+  </si>
+  <si>
+    <t>Disney's Mulan | Big Game Sneak Peek</t>
+  </si>
+  <si>
+    <t>Walt Disney Studios</t>
+  </si>
+  <si>
+    <t>Walt Disney</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=D1dnw4t23P8&amp;ab_channel=PrimeVideo</t>
+  </si>
+  <si>
+    <t>Hunters Super Bowl Trailers | Prime Video</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=m4sVnOsXlAA&amp;ab_channel=DonaldJTrump</t>
+  </si>
+  <si>
+    <t>Donald Trump</t>
+  </si>
+  <si>
+    <t>SUPER BOWL AD: Stronger, Safer, More Prosperous</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9Yp0yN8UxVg&amp;ab_channel=MikeBloomberg</t>
+  </si>
+  <si>
+    <t>Mike Bloomberg</t>
+  </si>
+  <si>
+    <t>SUPER BOWL AD: George | Mike Bloomberg for President</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=B5lslSPfhkg&amp;ab_channel=Dashlane</t>
+  </si>
+  <si>
+    <t>Password Paradise | Dashlane™ Big Game Commercial 2020</t>
+  </si>
+  <si>
+    <t>Dashlane</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cXw4sQJINgo&amp;ab_channel=Heinz</t>
+  </si>
+  <si>
+    <t>Heinz</t>
+  </si>
+  <si>
+    <t>Heinz - Find The Goodness - Four at Once</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Cdpf1Dl5b_4&amp;ab_channel=Cheetos</t>
+  </si>
+  <si>
+    <t>Cheetos® | Can't Touch This | SUPER BOWL LIV OFFICIAL VIDEO</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tHoYKy1GMgM&amp;ab_channel=MountainDew</t>
+  </si>
+  <si>
+    <t>MTN DEW Zero Sugar, As Good As The Original</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=U7h6Vls-uO8&amp;ab_channel=MichelobULTRA</t>
+  </si>
+  <si>
+    <t>Jimmy Works It Out | Michelob ULTRA | Super Bowl LIV</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ANarZ_113Xc&amp;ab_channel=MichelobULTRA</t>
+  </si>
+  <si>
+    <t>6 for 6-Pack | Michelob ULTRA Pure Gold | Super Bowl LIV</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gckObDeYpAA&amp;ab_channel=WeatherTech</t>
+  </si>
+  <si>
+    <t>Lucky Dog: 2020 WeatherTech Super Bowl Commercial</t>
   </si>
 </sst>
 </file>
@@ -1257,10 +1677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EDA2698-6B55-6F46-8306-C54161FB3AF5}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3037,6 +3457,958 @@
       </c>
       <c r="E104">
         <v>2023</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>277</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" t="s">
+        <v>278</v>
+      </c>
+      <c r="E105">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>279</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" t="s">
+        <v>280</v>
+      </c>
+      <c r="E106">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>281</v>
+      </c>
+      <c r="B107" t="s">
+        <v>282</v>
+      </c>
+      <c r="C107" t="s">
+        <v>282</v>
+      </c>
+      <c r="D107" t="s">
+        <v>283</v>
+      </c>
+      <c r="E107">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>285</v>
+      </c>
+      <c r="B108" t="s">
+        <v>147</v>
+      </c>
+      <c r="C108" t="s">
+        <v>149</v>
+      </c>
+      <c r="D108" t="s">
+        <v>284</v>
+      </c>
+      <c r="E108">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>287</v>
+      </c>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="s">
+        <v>286</v>
+      </c>
+      <c r="E109">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>288</v>
+      </c>
+      <c r="B110" t="s">
+        <v>291</v>
+      </c>
+      <c r="C110" t="s">
+        <v>290</v>
+      </c>
+      <c r="D110" t="s">
+        <v>289</v>
+      </c>
+      <c r="E110">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>295</v>
+      </c>
+      <c r="B111" t="s">
+        <v>294</v>
+      </c>
+      <c r="C111" t="s">
+        <v>293</v>
+      </c>
+      <c r="D111" t="s">
+        <v>292</v>
+      </c>
+      <c r="E111">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>297</v>
+      </c>
+      <c r="B112" t="s">
+        <v>298</v>
+      </c>
+      <c r="C112" t="s">
+        <v>298</v>
+      </c>
+      <c r="D112" t="s">
+        <v>296</v>
+      </c>
+      <c r="E112">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>299</v>
+      </c>
+      <c r="B113" t="s">
+        <v>301</v>
+      </c>
+      <c r="C113" t="s">
+        <v>301</v>
+      </c>
+      <c r="D113" t="s">
+        <v>300</v>
+      </c>
+      <c r="E113">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>303</v>
+      </c>
+      <c r="B114" t="s">
+        <v>64</v>
+      </c>
+      <c r="C114" t="s">
+        <v>65</v>
+      </c>
+      <c r="D114" t="s">
+        <v>302</v>
+      </c>
+      <c r="E114">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>305</v>
+      </c>
+      <c r="B115" t="s">
+        <v>63</v>
+      </c>
+      <c r="C115" t="s">
+        <v>62</v>
+      </c>
+      <c r="D115" t="s">
+        <v>304</v>
+      </c>
+      <c r="E115">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>307</v>
+      </c>
+      <c r="B116" t="s">
+        <v>257</v>
+      </c>
+      <c r="C116" t="s">
+        <v>93</v>
+      </c>
+      <c r="D116" t="s">
+        <v>306</v>
+      </c>
+      <c r="E116">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>309</v>
+      </c>
+      <c r="B117" t="s">
+        <v>108</v>
+      </c>
+      <c r="C117" t="s">
+        <v>108</v>
+      </c>
+      <c r="D117" t="s">
+        <v>308</v>
+      </c>
+      <c r="E117">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>312</v>
+      </c>
+      <c r="B118" t="s">
+        <v>311</v>
+      </c>
+      <c r="C118" t="s">
+        <v>311</v>
+      </c>
+      <c r="D118" t="s">
+        <v>310</v>
+      </c>
+      <c r="E118">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>314</v>
+      </c>
+      <c r="B119" t="s">
+        <v>147</v>
+      </c>
+      <c r="C119" t="s">
+        <v>149</v>
+      </c>
+      <c r="D119" t="s">
+        <v>313</v>
+      </c>
+      <c r="E119">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>315</v>
+      </c>
+      <c r="B120" t="s">
+        <v>316</v>
+      </c>
+      <c r="C120" t="s">
+        <v>316</v>
+      </c>
+      <c r="D120" t="s">
+        <v>317</v>
+      </c>
+      <c r="E120">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>319</v>
+      </c>
+      <c r="B121" t="s">
+        <v>46</v>
+      </c>
+      <c r="C121" t="s">
+        <v>46</v>
+      </c>
+      <c r="D121" t="s">
+        <v>318</v>
+      </c>
+      <c r="E121">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>322</v>
+      </c>
+      <c r="B122" t="s">
+        <v>321</v>
+      </c>
+      <c r="C122" t="s">
+        <v>103</v>
+      </c>
+      <c r="D122" t="s">
+        <v>320</v>
+      </c>
+      <c r="E122">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>324</v>
+      </c>
+      <c r="B123" t="s">
+        <v>264</v>
+      </c>
+      <c r="C123" t="s">
+        <v>264</v>
+      </c>
+      <c r="D123" t="s">
+        <v>323</v>
+      </c>
+      <c r="E123">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>326</v>
+      </c>
+      <c r="B124" t="s">
+        <v>327</v>
+      </c>
+      <c r="C124" t="s">
+        <v>327</v>
+      </c>
+      <c r="D124" t="s">
+        <v>325</v>
+      </c>
+      <c r="E124">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>330</v>
+      </c>
+      <c r="B125" t="s">
+        <v>329</v>
+      </c>
+      <c r="C125" t="s">
+        <v>329</v>
+      </c>
+      <c r="D125" t="s">
+        <v>328</v>
+      </c>
+      <c r="E125">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>333</v>
+      </c>
+      <c r="B126" t="s">
+        <v>332</v>
+      </c>
+      <c r="C126" t="s">
+        <v>332</v>
+      </c>
+      <c r="D126" t="s">
+        <v>331</v>
+      </c>
+      <c r="E126">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>335</v>
+      </c>
+      <c r="B127" t="s">
+        <v>67</v>
+      </c>
+      <c r="C127" t="s">
+        <v>67</v>
+      </c>
+      <c r="D127" t="s">
+        <v>334</v>
+      </c>
+      <c r="E127">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>337</v>
+      </c>
+      <c r="B128" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" t="s">
+        <v>336</v>
+      </c>
+      <c r="E128">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>339</v>
+      </c>
+      <c r="B129" t="s">
+        <v>76</v>
+      </c>
+      <c r="C129" t="s">
+        <v>76</v>
+      </c>
+      <c r="D129" t="s">
+        <v>338</v>
+      </c>
+      <c r="E129">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>341</v>
+      </c>
+      <c r="B130" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" t="s">
+        <v>340</v>
+      </c>
+      <c r="E130">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>343</v>
+      </c>
+      <c r="B131" t="s">
+        <v>344</v>
+      </c>
+      <c r="C131" t="s">
+        <v>344</v>
+      </c>
+      <c r="D131" t="s">
+        <v>342</v>
+      </c>
+      <c r="E131">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>346</v>
+      </c>
+      <c r="B132" t="s">
+        <v>147</v>
+      </c>
+      <c r="C132" t="s">
+        <v>149</v>
+      </c>
+      <c r="D132" t="s">
+        <v>345</v>
+      </c>
+      <c r="E132">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>349</v>
+      </c>
+      <c r="B133" t="s">
+        <v>348</v>
+      </c>
+      <c r="C133" t="s">
+        <v>348</v>
+      </c>
+      <c r="D133" t="s">
+        <v>347</v>
+      </c>
+      <c r="E133">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>351</v>
+      </c>
+      <c r="B134" t="s">
+        <v>257</v>
+      </c>
+      <c r="C134" t="s">
+        <v>93</v>
+      </c>
+      <c r="D134" t="s">
+        <v>350</v>
+      </c>
+      <c r="E134">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>353</v>
+      </c>
+      <c r="B135" t="s">
+        <v>234</v>
+      </c>
+      <c r="C135" t="s">
+        <v>234</v>
+      </c>
+      <c r="D135" t="s">
+        <v>352</v>
+      </c>
+      <c r="E135">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>355</v>
+      </c>
+      <c r="B136" t="s">
+        <v>356</v>
+      </c>
+      <c r="C136" t="s">
+        <v>356</v>
+      </c>
+      <c r="D136" t="s">
+        <v>354</v>
+      </c>
+      <c r="E136">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>358</v>
+      </c>
+      <c r="B137" t="s">
+        <v>187</v>
+      </c>
+      <c r="C137" t="s">
+        <v>187</v>
+      </c>
+      <c r="D137" t="s">
+        <v>357</v>
+      </c>
+      <c r="E137">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>360</v>
+      </c>
+      <c r="B138" t="s">
+        <v>264</v>
+      </c>
+      <c r="C138" t="s">
+        <v>264</v>
+      </c>
+      <c r="D138" t="s">
+        <v>359</v>
+      </c>
+      <c r="E138">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>362</v>
+      </c>
+      <c r="B139" t="s">
+        <v>264</v>
+      </c>
+      <c r="C139" t="s">
+        <v>264</v>
+      </c>
+      <c r="D139" t="s">
+        <v>361</v>
+      </c>
+      <c r="E139">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>364</v>
+      </c>
+      <c r="B140" t="s">
+        <v>147</v>
+      </c>
+      <c r="C140" t="s">
+        <v>149</v>
+      </c>
+      <c r="D140" t="s">
+        <v>363</v>
+      </c>
+      <c r="E140">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>366</v>
+      </c>
+      <c r="B141" t="s">
+        <v>367</v>
+      </c>
+      <c r="C141" t="s">
+        <v>368</v>
+      </c>
+      <c r="D141" t="s">
+        <v>365</v>
+      </c>
+      <c r="E141">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>370</v>
+      </c>
+      <c r="B142" t="s">
+        <v>294</v>
+      </c>
+      <c r="C142" t="s">
+        <v>293</v>
+      </c>
+      <c r="D142" t="s">
+        <v>369</v>
+      </c>
+      <c r="E142">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>373</v>
+      </c>
+      <c r="B143" t="s">
+        <v>372</v>
+      </c>
+      <c r="C143" t="s">
+        <v>374</v>
+      </c>
+      <c r="D143" t="s">
+        <v>371</v>
+      </c>
+      <c r="E143">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>377</v>
+      </c>
+      <c r="B144" t="s">
+        <v>376</v>
+      </c>
+      <c r="C144" t="s">
+        <v>376</v>
+      </c>
+      <c r="D144" t="s">
+        <v>375</v>
+      </c>
+      <c r="E144">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>379</v>
+      </c>
+      <c r="B145" t="s">
+        <v>294</v>
+      </c>
+      <c r="C145" t="s">
+        <v>293</v>
+      </c>
+      <c r="D145" t="s">
+        <v>378</v>
+      </c>
+      <c r="E145">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>381</v>
+      </c>
+      <c r="B146" t="s">
+        <v>224</v>
+      </c>
+      <c r="C146" t="s">
+        <v>224</v>
+      </c>
+      <c r="D146" t="s">
+        <v>380</v>
+      </c>
+      <c r="E146">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>383</v>
+      </c>
+      <c r="B147" t="s">
+        <v>16</v>
+      </c>
+      <c r="C147" t="s">
+        <v>16</v>
+      </c>
+      <c r="D147" t="s">
+        <v>382</v>
+      </c>
+      <c r="E147">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>386</v>
+      </c>
+      <c r="B148" t="s">
+        <v>385</v>
+      </c>
+      <c r="C148" t="s">
+        <v>385</v>
+      </c>
+      <c r="D148" t="s">
+        <v>384</v>
+      </c>
+      <c r="E148">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>388</v>
+      </c>
+      <c r="B149" t="s">
+        <v>16</v>
+      </c>
+      <c r="C149" t="s">
+        <v>16</v>
+      </c>
+      <c r="D149" t="s">
+        <v>387</v>
+      </c>
+      <c r="E149">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>390</v>
+      </c>
+      <c r="B150" t="s">
+        <v>391</v>
+      </c>
+      <c r="C150" t="s">
+        <v>392</v>
+      </c>
+      <c r="D150" t="s">
+        <v>389</v>
+      </c>
+      <c r="E150">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>394</v>
+      </c>
+      <c r="B151" t="s">
+        <v>282</v>
+      </c>
+      <c r="C151" t="s">
+        <v>282</v>
+      </c>
+      <c r="D151" t="s">
+        <v>393</v>
+      </c>
+      <c r="E151">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>397</v>
+      </c>
+      <c r="B152" t="s">
+        <v>396</v>
+      </c>
+      <c r="C152" t="s">
+        <v>396</v>
+      </c>
+      <c r="D152" t="s">
+        <v>395</v>
+      </c>
+      <c r="E152">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>400</v>
+      </c>
+      <c r="B153" t="s">
+        <v>399</v>
+      </c>
+      <c r="C153" t="s">
+        <v>399</v>
+      </c>
+      <c r="D153" t="s">
+        <v>398</v>
+      </c>
+      <c r="E153">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>402</v>
+      </c>
+      <c r="B154" t="s">
+        <v>403</v>
+      </c>
+      <c r="C154" t="s">
+        <v>403</v>
+      </c>
+      <c r="D154" t="s">
+        <v>401</v>
+      </c>
+      <c r="E154">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>406</v>
+      </c>
+      <c r="B155" t="s">
+        <v>405</v>
+      </c>
+      <c r="C155" t="s">
+        <v>405</v>
+      </c>
+      <c r="D155" t="s">
+        <v>404</v>
+      </c>
+      <c r="E155">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>408</v>
+      </c>
+      <c r="B156" t="s">
+        <v>301</v>
+      </c>
+      <c r="C156" t="s">
+        <v>301</v>
+      </c>
+      <c r="D156" t="s">
+        <v>407</v>
+      </c>
+      <c r="E156">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>410</v>
+      </c>
+      <c r="B157" t="s">
+        <v>76</v>
+      </c>
+      <c r="C157" t="s">
+        <v>76</v>
+      </c>
+      <c r="D157" t="s">
+        <v>409</v>
+      </c>
+      <c r="E157">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>412</v>
+      </c>
+      <c r="B158" t="s">
+        <v>147</v>
+      </c>
+      <c r="C158" t="s">
+        <v>149</v>
+      </c>
+      <c r="D158" t="s">
+        <v>411</v>
+      </c>
+      <c r="E158">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>414</v>
+      </c>
+      <c r="B159" t="s">
+        <v>147</v>
+      </c>
+      <c r="C159" t="s">
+        <v>149</v>
+      </c>
+      <c r="D159" t="s">
+        <v>413</v>
+      </c>
+      <c r="E159">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>416</v>
+      </c>
+      <c r="B160" t="s">
+        <v>264</v>
+      </c>
+      <c r="C160" t="s">
+        <v>264</v>
+      </c>
+      <c r="D160" t="s">
+        <v>415</v>
+      </c>
+      <c r="E160">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>